<commit_message>
After successfully writing viewByObject method in ViewControl class to select view to edit.
</commit_message>
<xml_diff>
--- a/resources/excelTestData.xlsx
+++ b/resources/excelTestData.xlsx
@@ -48,15 +48,9 @@
     <t>viewName</t>
   </si>
   <si>
-    <t>Test_Cloned</t>
-  </si>
-  <si>
     <t>newViewName</t>
   </si>
   <si>
-    <t>Test_Cloned_Edited</t>
-  </si>
-  <si>
     <t>columnsToSelect</t>
   </si>
   <si>
@@ -67,6 +61,12 @@
   </si>
   <si>
     <t>Source, Includes, Orcl_dvSum</t>
+  </si>
+  <si>
+    <t>testView</t>
+  </si>
+  <si>
+    <t>testViewEdited</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,27 +409,27 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After successfully writing getByObjectFromString method in EditViewForm class to select columns.
</commit_message>
<xml_diff>
--- a/resources/excelTestData.xlsx
+++ b/resources/excelTestData.xlsx
@@ -63,10 +63,10 @@
     <t>Source, Includes, Orcl_dvSum</t>
   </si>
   <si>
-    <t>testView</t>
-  </si>
-  <si>
-    <t>testViewEdited</t>
+    <t>testViewTwo</t>
+  </si>
+  <si>
+    <t>testViewTwoEdited</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
After final refactor and removing commented code.
</commit_message>
<xml_diff>
--- a/resources/excelTestData.xlsx
+++ b/resources/excelTestData.xlsx
@@ -465,24 +465,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>